<commit_message>
added visualizations for dataset breakdown
</commit_message>
<xml_diff>
--- a/results/hate_speech_metrics.xlsx
+++ b/results/hate_speech_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>Positive_Occurrences</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline Accuracy</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +491,9 @@
       <c r="F2" t="n">
         <v>19330</v>
       </c>
+      <c r="G2" t="n">
+        <v>0.7129947253882188</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -508,6 +516,9 @@
       <c r="F3" t="n">
         <v>17883</v>
       </c>
+      <c r="G3" t="n">
+        <v>0.6596215558260484</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -530,6 +541,9 @@
       <c r="F4" t="n">
         <v>16760</v>
       </c>
+      <c r="G4" t="n">
+        <v>0.6181992549149792</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -552,6 +566,9 @@
       <c r="F5" t="n">
         <v>15709</v>
       </c>
+      <c r="G5" t="n">
+        <v>0.5794327025930435</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -574,6 +591,9 @@
       <c r="F6" t="n">
         <v>13949</v>
       </c>
+      <c r="G6" t="n">
+        <v>0.5145144037475563</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -596,6 +616,9 @@
       <c r="F7" t="n">
         <v>13877</v>
       </c>
+      <c r="G7" t="n">
+        <v>0.5118586551584228</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -618,6 +641,9 @@
       <c r="F8" t="n">
         <v>10165</v>
       </c>
+      <c r="G8" t="n">
+        <v>0.6250599387702409</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -640,6 +666,9 @@
       <c r="F9" t="n">
         <v>9821</v>
       </c>
+      <c r="G9" t="n">
+        <v>0.6377485153627679</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -662,6 +691,9 @@
       <c r="F10" t="n">
         <v>9278</v>
       </c>
+      <c r="G10" t="n">
+        <v>0.6577772859724835</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -684,6 +716,9 @@
       <c r="F11" t="n">
         <v>4928</v>
       </c>
+      <c r="G11" t="n">
+        <v>0.8182287632326362</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -705,6 +740,9 @@
       </c>
       <c r="F12" t="n">
         <v>2897</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.8931430046844454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>